<commit_message>
[TEST] : modif fichier test
</commit_message>
<xml_diff>
--- a/src/main/resources/testFiles/fichierTest.xlsx
+++ b/src/main/resources/testFiles/fichierTest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DEV\Projets\workspace\calcul-assmat-api\src\main\resources\testFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D8476EE-0940-4D65-8DA7-DAE7276935F1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8067DB0C-2565-47E5-A834-55C42E843E41}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,12 +16,12 @@
     <sheet name="Réponses au formulaire 1" sheetId="1" r:id="rId1"/>
     <sheet name="Feuille 1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="15">
   <si>
     <t>Horodateur</t>
   </si>
@@ -106,13 +106,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="19" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -430,11 +429,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
+      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -472,9 +471,6 @@
       <c r="A2" s="1">
         <v>43346.79166195602</v>
       </c>
-      <c r="B2" s="5">
-        <v>43346</v>
-      </c>
       <c r="C2" s="3" t="s">
         <v>10</v>
       </c>
@@ -489,9 +485,6 @@
       <c r="A3" s="1">
         <v>43346.791892789348</v>
       </c>
-      <c r="B3" s="5">
-        <v>43346</v>
-      </c>
       <c r="C3" s="3" t="s">
         <v>10</v>
       </c>
@@ -600,9 +593,6 @@
       <c r="A9" s="1">
         <v>43350.783746875</v>
       </c>
-      <c r="B9" s="2">
-        <v>43350</v>
-      </c>
       <c r="C9" s="3" t="s">
         <v>8</v>
       </c>
@@ -694,6 +684,77 @@
       </c>
       <c r="G13" s="3" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>43356.868058912034</v>
+      </c>
+      <c r="B14" s="2">
+        <v>43356</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="4">
+        <v>0.32291666666424135</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>43356.868448819441</v>
+      </c>
+      <c r="B15" s="2">
+        <v>43356</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" s="4">
+        <v>0.72916666666424135</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>43357.862597106483</v>
+      </c>
+      <c r="B16" s="2">
+        <v>43357</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="4">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>43357.862827986115</v>
+      </c>
+      <c r="B17" s="2">
+        <v>43357</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" s="4">
+        <v>0.70833333333575865</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[TESTS] : init TU + fichier test intégration
</commit_message>
<xml_diff>
--- a/src/main/resources/testFiles/fichierTest.xlsx
+++ b/src/main/resources/testFiles/fichierTest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DEV\Projets\workspace\calcul-assmat-api\src\main\resources\testFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8067DB0C-2565-47E5-A834-55C42E843E41}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8FE699A-BD13-4AF2-8C8D-0EEB5A06ECB6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="15">
   <si>
     <t>Horodateur</t>
   </si>
@@ -106,12 +106,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="19" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -429,11 +430,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
+      <selection pane="bottomLeft" activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -471,6 +472,9 @@
       <c r="A2" s="1">
         <v>43346.79166195602</v>
       </c>
+      <c r="B2" s="5">
+        <v>43346</v>
+      </c>
       <c r="C2" s="3" t="s">
         <v>10</v>
       </c>
@@ -485,6 +489,9 @@
       <c r="A3" s="1">
         <v>43346.791892789348</v>
       </c>
+      <c r="B3" s="5">
+        <v>43346</v>
+      </c>
       <c r="C3" s="3" t="s">
         <v>10</v>
       </c>
@@ -593,6 +600,9 @@
       <c r="A9" s="1">
         <v>43350.783746875</v>
       </c>
+      <c r="B9" s="2">
+        <v>43350</v>
+      </c>
       <c r="C9" s="3" t="s">
         <v>8</v>
       </c>
@@ -740,7 +750,7 @@
         <v>0.375</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>43357.862827986115</v>
       </c>
@@ -755,6 +765,43 @@
       </c>
       <c r="E17" s="4">
         <v>0.70833333333575865</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>43360.939879560188</v>
+      </c>
+      <c r="B18" s="2">
+        <v>43360</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" s="4">
+        <v>0.32291666666424135</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>43360.940077534724</v>
+      </c>
+      <c r="B19" s="2">
+        <v>43360</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" s="4">
+        <v>0.70833333333575865</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[SYNTHESE] : avancement du calcul
</commit_message>
<xml_diff>
--- a/src/main/resources/testFiles/fichierTest.xlsx
+++ b/src/main/resources/testFiles/fichierTest.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DEV\Projets\workspace\calcul-assmat-api\src\main\resources\testFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\formation-workspaces\calcul-assmat-api\src\main\resources\testFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8FE699A-BD13-4AF2-8C8D-0EEB5A06ECB6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Réponses au formulaire 1" sheetId="1" r:id="rId1"/>
@@ -21,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="15">
   <si>
     <t>Horodateur</t>
   </si>
@@ -71,7 +70,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm:ss"/>
   </numFmts>
@@ -147,7 +146,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -159,7 +158,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -206,23 +205,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -258,23 +240,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -426,23 +391,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B24" sqref="B24"/>
+      <selection pane="bottomLeft" activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="14" width="21.5546875" customWidth="1"/>
+    <col min="1" max="14" width="21.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -468,7 +433,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>43346.79166195602</v>
       </c>
@@ -485,7 +450,7 @@
         <v>0.38541666666424135</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>43346.791892789348</v>
       </c>
@@ -502,7 +467,7 @@
         <v>0.70833333333575865</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>43347.328665138892</v>
       </c>
@@ -519,7 +484,7 @@
         <v>0.32291666666424135</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>43347.794715173615</v>
       </c>
@@ -542,7 +507,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>43349.921830497682</v>
       </c>
@@ -559,7 +524,7 @@
         <v>0.32291666666424135</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>43349.922125462967</v>
       </c>
@@ -579,7 +544,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>43350.783449976851</v>
       </c>
@@ -596,7 +561,7 @@
         <v>0.375</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>43350.783746875</v>
       </c>
@@ -619,7 +584,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>43353.883479074073</v>
       </c>
@@ -642,7 +607,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>43353.883786770835</v>
       </c>
@@ -659,7 +624,7 @@
         <v>0.71875</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>43354.774429189813</v>
       </c>
@@ -676,7 +641,7 @@
         <v>0.32291666666424135</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>43354.790583796297</v>
       </c>
@@ -696,7 +661,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>43356.868058912034</v>
       </c>
@@ -713,7 +678,7 @@
         <v>0.32291666666424135</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>43356.868448819441</v>
       </c>
@@ -733,7 +698,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>43357.862597106483</v>
       </c>
@@ -750,7 +715,7 @@
         <v>0.375</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>43357.862827986115</v>
       </c>
@@ -767,7 +732,7 @@
         <v>0.70833333333575865</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>43360.939879560188</v>
       </c>
@@ -784,7 +749,7 @@
         <v>0.32291666666424135</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>43360.940077534724</v>
       </c>
@@ -801,6 +766,154 @@
         <v>0.70833333333575865</v>
       </c>
       <c r="G19" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <v>43361.832989317132</v>
+      </c>
+      <c r="B20" s="2">
+        <v>43361</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" s="4">
+        <v>0.32291666666424135</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <v>43361.833331574075</v>
+      </c>
+      <c r="B21" s="2">
+        <v>43361</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" s="4">
+        <v>0.73958333333575865</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
+        <v>43363.782638321762</v>
+      </c>
+      <c r="B22" s="2">
+        <v>43363</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E22" s="4">
+        <v>0.32291666666424135</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
+        <v>43363.782996678245</v>
+      </c>
+      <c r="B23" s="2">
+        <v>43363</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E23" s="4">
+        <v>0.71875</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
+        <v>43364.972090138894</v>
+      </c>
+      <c r="B24" s="2">
+        <v>43364</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" s="4">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
+        <v>43364.972291122685</v>
+      </c>
+      <c r="B25" s="2">
+        <v>43364</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E25" s="4">
+        <v>0.73958333333575865</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
+        <v>43367.817552430555</v>
+      </c>
+      <c r="B26" s="2">
+        <v>43367</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26" s="4">
+        <v>0.32291666666424135</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
+        <v>43367.817830601853</v>
+      </c>
+      <c r="B27" s="2">
+        <v>43367</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E27" s="4">
+        <v>0.72916666666424135</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G27" s="3" t="s">
         <v>12</v>
       </c>
     </row>
@@ -810,7 +923,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -818,7 +931,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>